<commit_message>
added a 11th week
</commit_message>
<xml_diff>
--- a/0_appendix/labeling/box_labels.xlsx
+++ b/0_appendix/labeling/box_labels.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="441">
   <si>
     <t xml:space="preserve">Date :  
 Code : T1-G1-I1-CA</t>
@@ -1615,6 +1615,166 @@
   <si>
     <t xml:space="preserve">Date :  
 Code : T5-G100-I400-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T1-G101-I401-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T1-G101-I402-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T1-G101-I403-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T1-G101-I404-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T1-G102-I405-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T1-G102-I406-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T1-G102-I407-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T1-G102-I408-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T2-G103-I409-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T2-G103-I410-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T2-G103-I411-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T2-G103-I412-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T2-G104-I413-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T2-G104-I414-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T2-G104-I415-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T2-G104-I416-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T3-G105-I417-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T3-G105-I418-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T3-G105-I419-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T3-G105-I420-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T3-G106-I421-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T3-G106-I422-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T3-G106-I423-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T3-G106-I424-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T4-G107-I425-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T4-G107-I426-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T4-G107-I427-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T4-G107-I428-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T4-G108-I429-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T4-G108-I430-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T4-G108-I431-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T4-G108-I432-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T5-G109-I433-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T5-G109-I434-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T5-G109-I435-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T5-G109-I436-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T5-G110-I437-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T5-G110-I438-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T5-G110-I439-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date :  
+Code : T5-G110-I440-EP</t>
   </si>
 </sst>
 </file>
@@ -4247,19 +4407,249 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101"/>
+      <c r="A101" t="s">
+        <v>401</v>
+      </c>
       <c r="B101" t="s">
         <v>1</v>
       </c>
-      <c r="C101"/>
+      <c r="C101" t="s">
+        <v>402</v>
+      </c>
       <c r="D101" t="s">
         <v>1</v>
       </c>
-      <c r="E101"/>
+      <c r="E101" t="s">
+        <v>403</v>
+      </c>
       <c r="F101" t="s">
         <v>1</v>
       </c>
-      <c r="G101"/>
+      <c r="G101" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>405</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>406</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>407</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1</v>
+      </c>
+      <c r="G102" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>409</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>410</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
+        <v>411</v>
+      </c>
+      <c r="F103" t="s">
+        <v>1</v>
+      </c>
+      <c r="G103" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>413</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>414</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1</v>
+      </c>
+      <c r="E104" t="s">
+        <v>415</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1</v>
+      </c>
+      <c r="G104" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>417</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>418</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1</v>
+      </c>
+      <c r="E105" t="s">
+        <v>419</v>
+      </c>
+      <c r="F105" t="s">
+        <v>1</v>
+      </c>
+      <c r="G105" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>421</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>422</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1</v>
+      </c>
+      <c r="E106" t="s">
+        <v>423</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1</v>
+      </c>
+      <c r="G106" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>425</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>426</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1</v>
+      </c>
+      <c r="E107" t="s">
+        <v>427</v>
+      </c>
+      <c r="F107" t="s">
+        <v>1</v>
+      </c>
+      <c r="G107" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>429</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" t="s">
+        <v>430</v>
+      </c>
+      <c r="D108" t="s">
+        <v>1</v>
+      </c>
+      <c r="E108" t="s">
+        <v>431</v>
+      </c>
+      <c r="F108" t="s">
+        <v>1</v>
+      </c>
+      <c r="G108" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>433</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>434</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
+        <v>435</v>
+      </c>
+      <c r="F109" t="s">
+        <v>1</v>
+      </c>
+      <c r="G109" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>437</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>438</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
+        <v>439</v>
+      </c>
+      <c r="F110" t="s">
+        <v>1</v>
+      </c>
+      <c r="G110" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111"/>
+      <c r="B111" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111"/>
+      <c r="D111" t="s">
+        <v>1</v>
+      </c>
+      <c r="E111"/>
+      <c r="F111" t="s">
+        <v>1</v>
+      </c>
+      <c r="G111"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>